<commit_message>
restructure results summary plots
</commit_message>
<xml_diff>
--- a/dataset_summary.xlsx
+++ b/dataset_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">nonlinear system of k=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_14_21</t>
   </si>
 </sst>
 </file>
@@ -223,10 +226,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,7 +434,8 @@
       <c r="D9" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E9" s="2" t="b">
+      <c r="E9" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -439,6 +443,23 @@
       </c>
       <c r="H9" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to diffusion/laplacian analysis
</commit_message>
<xml_diff>
--- a/dataset_summary.xlsx
+++ b/dataset_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -175,7 +175,10 @@
     <t xml:space="preserve">Rand [-1, 1]</t>
   </si>
   <si>
-    <t xml:space="preserve">01_18_22</t>
+    <t xml:space="preserve">01_19_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
   </si>
 </sst>
 </file>
@@ -315,10 +318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -851,32 +854,23 @@
       <c r="A22" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="D22" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E22" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1000000</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
+        <v>2000</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
ArgparseConverter class in argparse_utils
</commit_message>
<xml_diff>
--- a/dataset_summary.xlsx
+++ b/dataset_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">Delete</t>
+  </si>
+  <si>
     <t xml:space="preserve">08_24_21</t>
   </si>
   <si>
@@ -151,6 +154,9 @@
     <t xml:space="preserve">1-2-3-4</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">01_14_22</t>
   </si>
   <si>
@@ -179,15 +185,29 @@
   </si>
   <si>
     <t xml:space="preserve">??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04_26_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2048 beads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04_27_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1024 beads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_12_22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -263,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,15 +292,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,21 +373,24 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -388,18 +403,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -407,26 +422,26 @@
         <v>500000</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -434,23 +449,23 @@
         <v>500000</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -460,35 +475,32 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+        <v>22</v>
+      </c>
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -498,18 +510,18 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -517,36 +529,36 @@
         <v>1000000</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3" t="n">
+    </row>
+    <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>28.7</v>
-      </c>
-      <c r="E9" s="4" t="n">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>28</v>
+      <c r="F9" s="2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>15</v>
@@ -554,7 +566,7 @@
       <c r="D10" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -562,26 +574,26 @@
         <v>1000000</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -589,23 +601,23 @@
         <v>1000000</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -613,23 +625,23 @@
         <v>1000000</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -637,23 +649,23 @@
         <v>1000000</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -661,23 +673,23 @@
         <v>1000000</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -685,23 +697,23 @@
         <v>1000000</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -709,50 +721,53 @@
         <v>1000000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>28.7</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>28</v>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -760,26 +775,29 @@
         <v>1000000</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -790,23 +808,23 @@
         <v>2000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -817,23 +835,26 @@
         <v>100</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>28.7</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -844,15 +865,15 @@
         <v>4000</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>28.7</v>
@@ -867,7 +888,85 @@
         <v>2000</v>
       </c>
       <c r="I22" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
various changes associated with switch to pylib
</commit_message>
<xml_diff>
--- a/dataset_summary.xlsx
+++ b/dataset_summary.xlsx
@@ -20,23 +20,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
   <si>
+    <t xml:space="preserve">experimental</t>
+  </si>
+  <si>
     <t xml:space="preserve">k</t>
   </si>
   <si>
     <t xml:space="preserve">chi</t>
   </si>
   <si>
+    <t xml:space="preserve">seq</t>
+  </si>
+  <si>
     <t xml:space="preserve">diag</t>
   </si>
   <si>
     <t xml:space="preserve">sweeps</t>
   </si>
   <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
@@ -55,6 +64,9 @@
     <t xml:space="preserve">[-1, 1], [1, 0]</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">max diag chi = 0.1</t>
   </si>
   <si>
@@ -113,6 +125,108 @@
   </si>
   <si>
     <t xml:space="preserve">05_12_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07_20_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_14_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_18_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_21_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_06_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_22_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_23_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_25_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_26_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_27_23_v9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_01_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_04_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_06_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_07_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_08_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_13_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_14_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_16_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_20_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_21_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_22_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_27_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_01_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_03_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_ent_v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_21_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixed experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_22_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_23_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_29_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04_04_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_ent_poly6_log_v2_grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04_06_23</t>
   </si>
 </sst>
 </file>
@@ -121,7 +235,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -189,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,11 +312,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,17 +354,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H1"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K1"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="dataset"/>
-    <tableColumn id="2" name="k"/>
-    <tableColumn id="3" name="chi"/>
-    <tableColumn id="4" name="diag"/>
-    <tableColumn id="5" name="sweeps"/>
-    <tableColumn id="6" name="N"/>
-    <tableColumn id="7" name="maxent samples"/>
-    <tableColumn id="8" name="Comments"/>
+    <tableColumn id="2" name="experimental"/>
+    <tableColumn id="3" name="k"/>
+    <tableColumn id="4" name="chi"/>
+    <tableColumn id="5" name="seq"/>
+    <tableColumn id="6" name="diag"/>
+    <tableColumn id="7" name="sweeps"/>
+    <tableColumn id="8" name="m"/>
+    <tableColumn id="9" name="N"/>
+    <tableColumn id="10" name="maxent samples"/>
+    <tableColumn id="11" name="Comments"/>
   </tableColumns>
 </table>
 </file>
@@ -256,22 +377,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="5.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,226 +421,436 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="n">
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>1000000</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>17</v>
+      <c r="K4" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="D5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>17</v>
+      <c r="K5" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="D6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
+      <c r="K6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
+      <c r="J7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="D8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>27</v>
+      <c r="K8" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="D9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>29</v>
+      <c r="K9" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="0" t="n">
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>1000000</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K10" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>500000</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>500000</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
bug fix in load_Y
</commit_message>
<xml_diff>
--- a/dataset_summary.xlsx
+++ b/dataset_summary.xlsx
@@ -303,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,14 +313,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,7 +372,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,7 +456,7 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="n">
@@ -484,7 +476,6 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4"/>
       <c r="G4" s="0" t="n">
         <v>1000000</v>
       </c>
@@ -502,7 +493,6 @@
       <c r="D5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4"/>
       <c r="G5" s="0" t="n">
         <v>1000000</v>
       </c>
@@ -520,7 +510,7 @@
       <c r="D6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="0" t="n">
@@ -543,7 +533,7 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -569,7 +559,7 @@
       <c r="D8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -592,7 +582,7 @@
       <c r="D9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="0" t="n">
@@ -615,7 +605,7 @@
       <c r="D10" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="0" t="n">
@@ -632,25 +622,21 @@
       <c r="A11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">

</xml_diff>